<commit_message>
Checked all externally needed parts.
</commit_message>
<xml_diff>
--- a/imu checklist.xlsx
+++ b/imu checklist.xlsx
@@ -73,30 +73,18 @@
     <t>.1uF cap on vddio</t>
   </si>
   <si>
-    <t>Additional filteringesistor or ferrite bead in series with VS no greater than 100ohm</t>
-  </si>
-  <si>
     <t>Increase bypass cap on vs to 10uF and .1uF in paralell</t>
   </si>
   <si>
-    <t>Rec that vs and vddio be separate supplies.</t>
-  </si>
-  <si>
     <t>mounted close to a hard mounting point</t>
   </si>
   <si>
-    <t>size traces to external caps to carry 1amp</t>
-  </si>
-  <si>
     <t>.22uF cap between setc and setp</t>
   </si>
   <si>
     <t>vddio, vdd, and s1 connected</t>
   </si>
   <si>
-    <t>.1uF between vddio(and othersin above cell) to gnd</t>
-  </si>
-  <si>
     <t>4.7uF cap on c1 to gnd (might need to be polarized)</t>
   </si>
   <si>
@@ -115,9 +103,6 @@
     <t>pb free solder</t>
   </si>
   <si>
-    <t>ref13.3 ref2 5v</t>
-  </si>
-  <si>
     <t>en to vref2, both pulled to 5v with 200kohm resistor</t>
   </si>
   <si>
@@ -139,9 +124,6 @@
     <t>1uF to 10uF cap on input if more than 6" from main input filter cap</t>
   </si>
   <si>
-    <t>at least 3.3uF solid tantalum cap on output ESR of 2ohm or less</t>
-  </si>
-  <si>
     <t>Avcc externally connected to vcc through low pass filter</t>
   </si>
   <si>
@@ -155,13 +137,32 @@
   </si>
   <si>
     <t>Extra:</t>
+  </si>
+  <si>
+    <t>size traces to external caps to carry 1amp (11mil)
+http://www.desmith.net/NMdS/Electronics/TraceWidth.html</t>
+  </si>
+  <si>
+    <t>.1uF between vddio(and others in above cell) to gnd</t>
+  </si>
+  <si>
+    <t>Recomended that vs and vddio be separate supplies.</t>
+  </si>
+  <si>
+    <t>Additional filtering resistor or ferrite bead in series with VS no greater than 100ohm</t>
+  </si>
+  <si>
+    <t>ref1 3.3 ref2 5v</t>
+  </si>
+  <si>
+    <t>at least 3.3uF solid tantalum? cap on output ESR of 2ohm or less</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,16 +185,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -254,11 +279,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -284,8 +326,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -603,10 +671,10 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -664,10 +732,10 @@
         <v>10</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>12</v>
@@ -676,114 +744,114 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>41</v>
+      <c r="G3" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>42</v>
+        <v>22</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>44</v>
+      <c r="C5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>35</v>
+      <c r="B6" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>36</v>
+      <c r="B7" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>27</v>
+      <c r="B8" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="5" t="s">
-        <v>21</v>
+      <c r="B9" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rechecked datasheets again, (found some errors highlighted in red, semi errors in yellow)
</commit_message>
<xml_diff>
--- a/imu checklist.xlsx
+++ b/imu checklist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="24" windowWidth="22980" windowHeight="9792"/>
+    <workbookView xWindow="0" yWindow="84" windowWidth="22980" windowHeight="9732"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,13 +67,7 @@
 </t>
   </si>
   <si>
-    <t>1uF cap on VS</t>
-  </si>
-  <si>
     <t>.1uF cap on vddio</t>
-  </si>
-  <si>
-    <t>Increase bypass cap on vs to 10uF and .1uF in paralell</t>
   </si>
   <si>
     <t>mounted close to a hard mounting point</t>
@@ -156,13 +150,19 @@
   </si>
   <si>
     <t>at least 3.3uF solid tantalum? cap on output ESR of 2ohm or less</t>
+  </si>
+  <si>
+    <t>1uF tantalum cap on VS</t>
+  </si>
+  <si>
+    <t>Increase bypass cap on vs to 10uF tantalum and .1uF ceramic in paralell</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,8 +199,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +230,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
   </fills>
@@ -295,12 +320,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -341,17 +368,22 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+    <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -674,7 +706,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -732,10 +764,10 @@
         <v>10</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>12</v>
@@ -746,112 +778,112 @@
     </row>
     <row r="3" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>43</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>22</v>
+      <c r="B4" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>20</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F4" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>34</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B7" s="12" t="s">
-        <v>18</v>
+    <row r="7" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="17" t="s">
+        <v>45</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B8" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>23</v>
+      <c r="B8" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Transitioned to the tantalum caps where needed (BOM,Checklist, and PCB)
</commit_message>
<xml_diff>
--- a/imu checklist.xlsx
+++ b/imu checklist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="84" windowWidth="22980" windowHeight="9732"/>
+    <workbookView xWindow="0" yWindow="144" windowWidth="22980" windowHeight="9672"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -79,9 +79,6 @@
     <t>vddio, vdd, and s1 connected</t>
   </si>
   <si>
-    <t>4.7uF cap on c1 to gnd (might need to be polarized)</t>
-  </si>
-  <si>
     <t>external caps should be ceramic and low esr (below 200mOhms)</t>
   </si>
   <si>
@@ -156,13 +153,38 @@
   </si>
   <si>
     <t>Increase bypass cap on vs to 10uF tantalum and .1uF ceramic in paralell</t>
+  </si>
+  <si>
+    <r>
+      <t>4.7uF cap on c1 to gnd (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>might need to be polarized)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> not pol because tant have high esr</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +236,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -243,7 +279,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -319,6 +355,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -327,7 +378,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -353,32 +404,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -706,7 +745,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -764,10 +803,10 @@
         <v>10</v>
       </c>
       <c r="F2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>12</v>
@@ -778,113 +817,138 @@
     </row>
     <row r="3" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="B4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3" s="10" t="s">
+      <c r="E4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>34</v>
-      </c>
+      <c r="I4" s="11"/>
     </row>
     <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>27</v>
-      </c>
+      <c r="D5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
       <c r="H5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="12" t="s">
-        <v>41</v>
+      <c r="B6" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>28</v>
-      </c>
+      <c r="D6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
     </row>
     <row r="7" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>29</v>
-      </c>
+      <c r="B7" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
     </row>
     <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B8" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>21</v>
-      </c>
+      <c r="B8" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
     </row>
     <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>17</v>
       </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:G1">

</xml_diff>

<commit_message>
Need 10uF cap on usbvccc, dont need lowpass on atmega8u2 because not using analog capabilities
</commit_message>
<xml_diff>
--- a/imu checklist.xlsx
+++ b/imu checklist.xlsx
@@ -4,19 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="144" windowWidth="22980" windowHeight="9672"/>
+    <workbookView xWindow="0" yWindow="204" windowWidth="22980" windowHeight="9612"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>ADXL345</t>
   </si>
@@ -179,12 +177,30 @@
       <t xml:space="preserve"> not pol because tant have high esr</t>
     </r>
   </si>
+  <si>
+    <t>10uF cap on usbvcc highly recommended</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Avcc externally connected to vcc through low pass filter  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Not using adc on the 8u2</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,6 +262,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -745,7 +768,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -837,8 +860,8 @@
       <c r="G3" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="10" t="s">
-        <v>32</v>
+      <c r="H3" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="I3" s="10" t="s">
         <v>32</v>
@@ -905,7 +928,9 @@
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="H6" s="11" t="s">
+        <v>46</v>
+      </c>
       <c r="I6" s="11"/>
     </row>
     <row r="7" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
@@ -962,28 +987,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Low Filteron 328p, and Cap on usbvcc are added
</commit_message>
<xml_diff>
--- a/imu checklist.xlsx
+++ b/imu checklist.xlsx
@@ -768,7 +768,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -863,7 +863,7 @@
       <c r="H3" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="9" t="s">
         <v>32</v>
       </c>
     </row>
@@ -928,7 +928,7 @@
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="9" t="s">
         <v>46</v>
       </c>
       <c r="I6" s="11"/>

</xml_diff>

<commit_message>
Everything accounted for except the hmc5883l caps need to be checked for low esr
</commit_message>
<xml_diff>
--- a/imu checklist.xlsx
+++ b/imu checklist.xlsx
@@ -151,6 +151,24 @@
   </si>
   <si>
     <t>Increase bypass cap on vs to 10uF tantalum and .1uF ceramic in paralell</t>
+  </si>
+  <si>
+    <t>10uF cap on usbvcc highly recommended</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Avcc externally connected to vcc through low pass filter  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Not using adc on the 8u2</t>
+    </r>
   </si>
   <si>
     <r>
@@ -174,25 +192,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> not pol because tant have high esr</t>
-    </r>
-  </si>
-  <si>
-    <t>10uF cap on usbvcc highly recommended</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Avcc externally connected to vcc through low pass filter  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Not using adc on the 8u2</t>
+      <t xml:space="preserve"> not pol because tant have high esr (Also sparkfun used tantalum and it didn’t work)</t>
     </r>
   </si>
 </sst>
@@ -768,7 +768,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -861,18 +861,18 @@
         <v>42</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B4" s="9" t="s">
         <v>43</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>22</v>
@@ -929,7 +929,7 @@
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
       <c r="H6" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I6" s="11"/>
     </row>
@@ -937,7 +937,7 @@
       <c r="B7" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D7" s="11"/>

</xml_diff>

<commit_message>
BRD cleanup, Moved to new Eagle 6 Format again, Reference Designators Updated in XLS files
</commit_message>
<xml_diff>
--- a/imu checklist.xlsx
+++ b/imu checklist.xlsx
@@ -4,17 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="204" windowWidth="22980" windowHeight="9612"/>
+    <workbookView xWindow="-1824" yWindow="3312" windowWidth="22980" windowHeight="9588" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Verified Parts" sheetId="1" r:id="rId1"/>
+    <sheet name="Verified Schematic" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Verified Schematic'!$C$4:$H$48</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="142">
   <si>
     <t>ADXL345</t>
   </si>
@@ -195,12 +199,294 @@
       <t xml:space="preserve"> not pol because tant have high esr (Also sparkfun used tantalum and it didn’t work)</t>
     </r>
   </si>
+  <si>
+    <t>Part number</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>PJ202A</t>
+  </si>
+  <si>
+    <t>5mm Barrel Jack power Connector</t>
+  </si>
+  <si>
+    <t>PPPC081LFBN-RC</t>
+  </si>
+  <si>
+    <t>Female headers</t>
+  </si>
+  <si>
+    <t>PPPC061LFBN-RC</t>
+  </si>
+  <si>
+    <t>PPPC021LFBN-RC</t>
+  </si>
+  <si>
+    <t>MI0805J102R-10</t>
+  </si>
+  <si>
+    <t>SMD EMI Suppression Ferrite Beads</t>
+  </si>
+  <si>
+    <t>3-axis gyro</t>
+  </si>
+  <si>
+    <t>PCA9306DCUR</t>
+  </si>
+  <si>
+    <t>Logic level Translator I2c</t>
+  </si>
+  <si>
+    <t>3-axis magnetometer</t>
+  </si>
+  <si>
+    <t>3-axis accelerometer</t>
+  </si>
+  <si>
+    <t>ATmega328P-AU</t>
+  </si>
+  <si>
+    <t>AVR MCU</t>
+  </si>
+  <si>
+    <t>ATMEGA8U2-MU</t>
+  </si>
+  <si>
+    <t>USB AVR interface</t>
+  </si>
+  <si>
+    <t>PTS525SM10SMTR LFS</t>
+  </si>
+  <si>
+    <t>SMD Tactile Switch</t>
+  </si>
+  <si>
+    <t>molex miniB usb through hole</t>
+  </si>
+  <si>
+    <t>MINISMDC050F-2</t>
+  </si>
+  <si>
+    <t>resettable 500mA fuse</t>
+  </si>
+  <si>
+    <t>CAT16-220J4LF</t>
+  </si>
+  <si>
+    <t>22R resistor network</t>
+  </si>
+  <si>
+    <t>CAY16-102J4LF</t>
+  </si>
+  <si>
+    <t>1k resistor network</t>
+  </si>
+  <si>
+    <t>CAY16-103J4LF</t>
+  </si>
+  <si>
+    <t>10k resistor network</t>
+  </si>
+  <si>
+    <t>ABM3B-16.000MHZ-B2-T</t>
+  </si>
+  <si>
+    <t>16 MHz SMD Crystal</t>
+  </si>
+  <si>
+    <t>AWSCR-16.00MTD-T</t>
+  </si>
+  <si>
+    <t>16 MHz SMD Resonator</t>
+  </si>
+  <si>
+    <t>5988130107F</t>
+  </si>
+  <si>
+    <t>Serial LED</t>
+  </si>
+  <si>
+    <t>5988170107F</t>
+  </si>
+  <si>
+    <t>Other LED</t>
+  </si>
+  <si>
+    <t>FDN306P</t>
+  </si>
+  <si>
+    <t>Power Select FET</t>
+  </si>
+  <si>
+    <t>PGB1010603MR</t>
+  </si>
+  <si>
+    <t>USB data line esd supress</t>
+  </si>
+  <si>
+    <t>LM358D</t>
+  </si>
+  <si>
+    <t>OP-Amp</t>
+  </si>
+  <si>
+    <t>609-3218-ND</t>
+  </si>
+  <si>
+    <t>Male Headers</t>
+  </si>
+  <si>
+    <t>C1608X7R1E103K</t>
+  </si>
+  <si>
+    <t>.01uF Cap</t>
+  </si>
+  <si>
+    <t>C1608X7R1C104K</t>
+  </si>
+  <si>
+    <t>.1uF Cap</t>
+  </si>
+  <si>
+    <t>C1608X7R1A224K</t>
+  </si>
+  <si>
+    <t>.22uF Cap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3225X7R1E106K </t>
+  </si>
+  <si>
+    <t>10uF Cap</t>
+  </si>
+  <si>
+    <t>C1608Y5V1A105Z</t>
+  </si>
+  <si>
+    <t>1uFCap</t>
+  </si>
+  <si>
+    <t>C1608X7R1H222K</t>
+  </si>
+  <si>
+    <t>2200pF Cap</t>
+  </si>
+  <si>
+    <t>06031A220KAT2A</t>
+  </si>
+  <si>
+    <t>22pF Cap</t>
+  </si>
+  <si>
+    <t>C2012X5R1E475K</t>
+  </si>
+  <si>
+    <t>4.7uF Cap</t>
+  </si>
+  <si>
+    <t>TPSA475K020R1800</t>
+  </si>
+  <si>
+    <t>4.7uF Tantalum Cap</t>
+  </si>
+  <si>
+    <t>RC0603FR-07200KL</t>
+  </si>
+  <si>
+    <t>200k Resistor</t>
+  </si>
+  <si>
+    <t>RC0603FR-071K5L</t>
+  </si>
+  <si>
+    <t>1.5k Resistor</t>
+  </si>
+  <si>
+    <t>CRCW06031K00FKEA</t>
+  </si>
+  <si>
+    <t>1k Resistor</t>
+  </si>
+  <si>
+    <t>CRCW06031M00FKEA</t>
+  </si>
+  <si>
+    <t>1M Resistor</t>
+  </si>
+  <si>
+    <t>SS14</t>
+  </si>
+  <si>
+    <t>Diode</t>
+  </si>
+  <si>
+    <t>3v3 Regulator</t>
+  </si>
+  <si>
+    <t>LT1129CST-5#PBF</t>
+  </si>
+  <si>
+    <t>TPSR105K020R6000</t>
+  </si>
+  <si>
+    <t>1uF tantalum Cap</t>
+  </si>
+  <si>
+    <t>LMK212BJ106KD-T</t>
+  </si>
+  <si>
+    <t>CK2125100M-T</t>
+  </si>
+  <si>
+    <t>10uH Inductor</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>LT1129CST-3.3#PBF</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>BRD VER</t>
+  </si>
+  <si>
+    <t>SCH VER</t>
+  </si>
+  <si>
+    <t>Moisture sensitive</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Change to C1210 module</t>
+  </si>
+  <si>
+    <t>Way biggerr than footprint</t>
+  </si>
+  <si>
+    <t>Maybe move away from avr1</t>
+  </si>
+  <si>
+    <t>change to 0603</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,6 +558,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -401,7 +692,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -442,6 +733,21 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -450,7 +756,42 @@
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -764,11 +1105,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -977,14 +1318,850 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:G1">
-    <cfRule type="expression" dxfId="1" priority="5">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>#REF!="yes"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>#REF!="no"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:H48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="8.88671875" style="18"/>
+    <col min="3" max="3" width="11.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.88671875" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C4" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C5" s="18">
+        <v>1</v>
+      </c>
+      <c r="D5" s="14">
+        <v>548190519</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C6" s="18">
+        <v>1</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C7" s="18">
+        <v>1</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C8" s="18">
+        <v>1</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C9" s="18">
+        <v>1</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C10" s="18">
+        <v>1</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C11" s="18">
+        <v>1</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C12" s="18">
+        <v>1</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C13" s="18">
+        <v>2</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C14" s="18">
+        <v>2</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C15" s="18">
+        <v>2</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C16" s="18">
+        <v>2</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C17" s="18">
+        <v>2</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C18" s="18">
+        <v>2</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C19" s="18">
+        <v>2</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C20" s="18">
+        <v>2</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C21" s="18">
+        <v>2</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C22" s="18">
+        <v>3</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C23" s="18">
+        <v>3</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C24" s="18">
+        <v>3</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C25" s="18">
+        <v>3</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C26" s="18">
+        <v>3</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C27" s="18">
+        <v>3</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C28" s="18">
+        <v>3</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C29" s="18">
+        <v>3</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G29" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C30" s="18">
+        <v>3</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G30" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="H30" s="18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C31" s="18">
+        <v>3</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G31" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C32" s="18">
+        <v>3</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G32" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C33" s="18">
+        <v>3</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G33" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C34" s="18">
+        <v>3</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="F34" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G34" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="H34" s="18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C35" s="18">
+        <v>3</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G35" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C36" s="18">
+        <v>3</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="F36" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G36" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C37" s="18">
+        <v>3</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F37" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G37" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C38" s="18">
+        <v>3</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G38" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C39" s="18">
+        <v>3</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G39" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C40" s="18">
+        <v>3</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G40" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C41" s="18">
+        <v>3</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F41" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G41" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="42" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C42" s="18">
+        <v>3</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F42" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G42" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="43" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C43" s="18">
+        <v>3</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F43" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G43" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="44" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C44" s="18">
+        <v>3</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="F44" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G44" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="45" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C45" s="18">
+        <v>3</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="F45" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G45" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C46" s="18">
+        <v>3</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="F46" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G46" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C47" s="18">
+        <v>3</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="F47" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G47" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="48" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C48" s="18">
+        <v>3</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="F48" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G48" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="C4:H48">
+    <sortState ref="C5:H48">
+      <sortCondition ref="C4:C48"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="C5:E49">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>AND($F5="Y", $G5="Y")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>OR(AND($F5="Y",$G5="N"),AND($F5="N",$G5="Y"))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>AND($F5="N",$G5="N")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5:G48">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>F5="y"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>F5="N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated BOM to reflect change in Resonator Cleaned Up Directory
</commit_message>
<xml_diff>
--- a/imu checklist.xlsx
+++ b/imu checklist.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-1824" yWindow="3312" windowWidth="22980" windowHeight="9588" activeTab="1"/>
+    <workbookView xWindow="-1824" yWindow="3312" windowWidth="22980" windowHeight="9588"/>
   </bookViews>
   <sheets>
-    <sheet name="Verified Parts" sheetId="1" r:id="rId1"/>
-    <sheet name="Verified Schematic" sheetId="2" r:id="rId2"/>
+    <sheet name="Misc" sheetId="3" r:id="rId1"/>
+    <sheet name="Verified Parts" sheetId="1" r:id="rId2"/>
+    <sheet name="Verified Schematic" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Verified Schematic'!$C$4:$H$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Verified Schematic'!$C$4:$H$48</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="205">
   <si>
     <t>ADXL345</t>
   </si>
@@ -481,12 +482,201 @@
   <si>
     <t>change to 0603</t>
   </si>
+  <si>
+    <t>Operating Voltage Range</t>
+  </si>
+  <si>
+    <t>Supply Current</t>
+  </si>
+  <si>
+    <t>SubCircuits</t>
+  </si>
+  <si>
+    <t>Part #</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>typ</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>Interupts</t>
+  </si>
+  <si>
+    <t>140 uA</t>
+  </si>
+  <si>
+    <t>Add interupt circuitry</t>
+  </si>
+  <si>
+    <t>HMC5883</t>
+  </si>
+  <si>
+    <t>740 uA</t>
+  </si>
+  <si>
+    <t>ITG-3200</t>
+  </si>
+  <si>
+    <t>6.5 mA</t>
+  </si>
+  <si>
+    <t>ATMega328</t>
+  </si>
+  <si>
+    <t>12 mA</t>
+  </si>
+  <si>
+    <t>I2C</t>
+  </si>
+  <si>
+    <t>Connect to AVR1</t>
+  </si>
+  <si>
+    <t>Give permanent I2C Address</t>
+  </si>
+  <si>
+    <t>logic lever conerter</t>
+  </si>
+  <si>
+    <t>resistors on scl sck to gnd?</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Things I need</t>
+  </si>
+  <si>
+    <t>Add the power regs from the arduino</t>
+  </si>
+  <si>
+    <t>solder paste</t>
+  </si>
+  <si>
+    <t>Check the caps</t>
+  </si>
+  <si>
+    <t>fine soldering tip</t>
+  </si>
+  <si>
+    <t>Add the two huge caps</t>
+  </si>
+  <si>
+    <t>Add Big Caps</t>
+  </si>
+  <si>
+    <t>Sensor</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Alt Address</t>
+  </si>
+  <si>
+    <t>*7 bit addr</t>
+  </si>
+  <si>
+    <t>regulate to 2.5 instead of 3.3</t>
+  </si>
+  <si>
+    <t>0x53</t>
+  </si>
+  <si>
+    <t>0x1d</t>
+  </si>
+  <si>
+    <t>Choose between power sources</t>
+  </si>
+  <si>
+    <t>0x68</t>
+  </si>
+  <si>
+    <t>0x69</t>
+  </si>
+  <si>
+    <t>110100X</t>
+  </si>
+  <si>
+    <t>regulate to 3.3v</t>
+  </si>
+  <si>
+    <t>0x1E</t>
+  </si>
+  <si>
+    <t>0011110</t>
+  </si>
+  <si>
+    <t>fix usb powering avr2</t>
+  </si>
+  <si>
+    <t>AVR2</t>
+  </si>
+  <si>
+    <t>Conect to ICSP</t>
+  </si>
+  <si>
+    <t>connect to avr1</t>
+  </si>
+  <si>
+    <t>AVR1</t>
+  </si>
+  <si>
+    <t>connect to iscp</t>
+  </si>
+  <si>
+    <t>Multplexer</t>
+  </si>
+  <si>
+    <t>Analog</t>
+  </si>
+  <si>
+    <t>Digital</t>
+  </si>
+  <si>
+    <t>Sensors</t>
+  </si>
+  <si>
+    <t>change to adxl346</t>
+  </si>
+  <si>
+    <t>chang to hmc5883</t>
+  </si>
+  <si>
+    <t>Other Updates</t>
+  </si>
+  <si>
+    <t>Smaller package for avr2</t>
+  </si>
+  <si>
+    <t>add ground pad beneath both avr</t>
+  </si>
+  <si>
+    <t>update crystal schematic</t>
+  </si>
+  <si>
+    <t>correct the led resistor values</t>
+  </si>
+  <si>
+    <t>change footprints of caps and resistors</t>
+  </si>
+  <si>
+    <t>correct the caps</t>
+  </si>
+  <si>
+    <t>add standoffs and fiducials</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -564,6 +754,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -593,7 +789,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -684,6 +880,114 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -692,7 +996,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -746,6 +1050,53 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1103,6 +1454,587 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:L46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B4" s="19"/>
+      <c r="C4" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
+      <c r="K4" s="25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="K5" s="32" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B6" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="34">
+        <v>2</v>
+      </c>
+      <c r="D6" s="35">
+        <v>2.5</v>
+      </c>
+      <c r="E6" s="35">
+        <v>3.6</v>
+      </c>
+      <c r="F6" s="36"/>
+      <c r="G6" s="37" t="s">
+        <v>150</v>
+      </c>
+      <c r="H6" s="38"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="39" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="34">
+        <v>2.16</v>
+      </c>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35">
+        <v>3.6</v>
+      </c>
+      <c r="F7" s="36"/>
+      <c r="G7" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="H7" s="38"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="40"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="C8" s="34">
+        <v>2.1</v>
+      </c>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35">
+        <v>3.6</v>
+      </c>
+      <c r="F8" s="36"/>
+      <c r="G8" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="H8" s="38"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="40"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B9" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" s="42">
+        <v>1.8</v>
+      </c>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43">
+        <v>5.5</v>
+      </c>
+      <c r="F9" s="44"/>
+      <c r="G9" s="45" t="s">
+        <v>157</v>
+      </c>
+      <c r="H9" s="46"/>
+      <c r="K9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B10" s="37"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="L10" s="39" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="L11" s="39" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="37"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="L12" s="39" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B13" s="37"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="L13" s="39" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B14" s="37"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="K14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B15" s="47" t="s">
+        <v>164</v>
+      </c>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="L15" s="39" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B16" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="L16" s="39" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B17" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="L17" s="39" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B18" s="37"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="L18" s="39" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B19" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="C19" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="D19" s="48" t="s">
+        <v>173</v>
+      </c>
+      <c r="E19" s="35"/>
+      <c r="F19" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="L19" s="39" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B20" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="49" t="s">
+        <v>176</v>
+      </c>
+      <c r="D20" s="49" t="s">
+        <v>177</v>
+      </c>
+      <c r="E20" s="35"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="37"/>
+      <c r="L20" s="39" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B21" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>179</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="E21" s="35"/>
+      <c r="F21" s="51" t="s">
+        <v>181</v>
+      </c>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="L21" s="39" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B22" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>183</v>
+      </c>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="50" t="s">
+        <v>184</v>
+      </c>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="L22" s="39" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B23" s="35"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B24" s="37"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="K24" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B25" s="37"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="L25" s="39" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B26" s="37"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="L26" s="39" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B27" s="37"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="K29" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B30" s="35"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="L30" s="39" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B31" s="35"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B32" s="35"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="K32" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B33" s="37"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
+      <c r="L33" s="52" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B34" s="37"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
+      <c r="L34" s="52" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B35" s="37"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
+      <c r="K35" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B36" s="37"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="37"/>
+      <c r="L36" s="39" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B37" s="37"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+      <c r="L37" s="39" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B38" s="37"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="37"/>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B39" s="37"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="37"/>
+      <c r="K39" s="25" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B40" s="37"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="37"/>
+      <c r="K40" s="39" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B41" s="37"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="37"/>
+      <c r="K41" s="39" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K42" s="39" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K43" s="39" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K44" s="39" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K45" s="39" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K46" s="39" t="s">
+        <v>204</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="F4:H4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1330,11 +2262,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>

</xml_diff>